<commit_message>
merging of loose carton and residentail pickup for QQ
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageProfile.xlsx
+++ b/testdata/FCfiles/qa/ManageProfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\testdata\FCfiles\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B318F63-F587-47C6-8937-B0D876B4DD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AD4109-3C31-4EB3-9E2B-D62F480436ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FF125F1C-9927-44E3-BE4C-8ED054D4B06E}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <t>Carrier</t>
   </si>
   <si>
-    <t>ABF Freight, BTX Global Logistics, Ceva,FC Test Carrier, UPS, FragilePAK</t>
+    <t>ABF Freight, Ceva, FC Test Carrier, UPS, FragilePAK</t>
   </si>
 </sst>
 </file>

</xml_diff>